<commit_message>
adding grouping to the main demo run
</commit_message>
<xml_diff>
--- a/src/main/resources/org/jxls/demo/guide/grouping_template.xlsx
+++ b/src/main/resources/org/jxls/demo/guide/grouping_template.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -578,7 +578,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>

</xml_diff>

<commit_message>
grouping improvements (fix issue#70)
</commit_message>
<xml_diff>
--- a/src/main/resources/org/jxls/demo/guide/grouping_template.xlsx
+++ b/src/main/resources/org/jxls/demo/guide/grouping_template.xlsx
@@ -67,7 +67,7 @@
             <charset val="238"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="employees" groupBy="name" groupOrder="asc" lastCell="D7")</t>
+jx:each(items="employees" var="nameGroup" groupBy="name" groupOrder="asc" lastCell="D7")</t>
         </r>
       </text>
     </comment>
@@ -93,7 +93,7 @@
             <charset val="238"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="_group.items" var="employee" lastCell="D6")</t>
+jx:each(items="nameGroup.items" var="employee" lastCell="D6")</t>
         </r>
       </text>
     </comment>
@@ -128,9 +128,6 @@
     <t>${employee.bonus}</t>
   </si>
   <si>
-    <t>${_group.item.name}</t>
-  </si>
-  <si>
     <t>GROUP BY EMPLOYEE NAME</t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t>Grand Total:</t>
+  </si>
+  <si>
+    <t>${nameGroup.item.name}</t>
   </si>
 </sst>
 </file>
@@ -617,23 +617,23 @@
   <sheetData>
     <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="8"/>
     </row>
     <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -666,7 +666,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="12">
         <f>SUM(C6)</f>
@@ -675,7 +675,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="14">
         <f>SUM(C7)</f>

</xml_diff>